<commit_message>
running full analysis without 3 measures
</commit_message>
<xml_diff>
--- a/projects/DC_analysis/PTool_Full_Analysis.xlsx
+++ b/projects/DC_analysis/PTool_Full_Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="3000" windowWidth="10296" windowHeight="2364" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="-12" yWindow="3000" windowWidth="10296" windowHeight="2364" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2405" uniqueCount="653">
   <si>
     <t>type</t>
   </si>
@@ -1516,9 +1516,6 @@
     <t>1.14.7</t>
   </si>
   <si>
-    <t>cluster1</t>
-  </si>
-  <si>
     <t>add_chilled_water_pump_differential_pressure_reset_controls</t>
   </si>
   <si>
@@ -2000,6 +1997,9 @@
   </si>
   <si>
     <t>Ptool_Full_Analysis</t>
+  </si>
+  <si>
+    <t>cluster6</t>
   </si>
 </sst>
 </file>
@@ -4101,9 +4101,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4121,6 +4118,9 @@
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1801">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6258,8 +6258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6328,7 +6328,7 @@
         <v>98</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>491</v>
+        <v>652</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>100</v>
@@ -6377,7 +6377,7 @@
         <v>86</v>
       </c>
       <c r="B9" s="24">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="31"/>
@@ -6399,7 +6399,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>99</v>
@@ -6694,9 +6694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z185"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6751,14 +6751,14 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -6854,24 +6854,24 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="60" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="60" t="s">
+    <row r="4" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="59" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="59" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="59" t="s">
         <v>245</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B5" s="30" t="s">
@@ -7406,28 +7406,28 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B22" s="56" t="s">
+    <row r="22" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B22" s="55" t="s">
         <v>318</v>
       </c>
-      <c r="C22" s="56" t="s">
-        <v>492</v>
-      </c>
-      <c r="D22" s="56" t="s">
+      <c r="C22" s="55" t="s">
+        <v>491</v>
+      </c>
+      <c r="D22" s="55" t="s">
         <v>319</v>
       </c>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="J22" s="58"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="59"/>
-      <c r="N22" s="59"/>
-      <c r="O22" s="59"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="58"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="29"/>
@@ -7470,20 +7470,20 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B24" s="56" t="s">
+    <row r="24" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B24" s="55" t="s">
         <v>321</v>
       </c>
-      <c r="C24" s="56" t="s">
-        <v>493</v>
-      </c>
-      <c r="D24" s="56" t="s">
+      <c r="C24" s="55" t="s">
+        <v>492</v>
+      </c>
+      <c r="D24" s="55" t="s">
         <v>322</v>
       </c>
-      <c r="E24" s="56" t="s">
+      <c r="E24" s="55" t="s">
         <v>46</v>
       </c>
     </row>
@@ -7528,28 +7528,28 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B26" s="56" t="s">
+    <row r="26" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B26" s="55" t="s">
         <v>285</v>
       </c>
-      <c r="C26" s="56" t="s">
-        <v>494</v>
-      </c>
-      <c r="D26" s="56" t="s">
+      <c r="C26" s="55" t="s">
+        <v>493</v>
+      </c>
+      <c r="D26" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="56" t="s">
+      <c r="E26" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="J26" s="58"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="29"/>
@@ -7592,20 +7592,20 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B28" s="56" t="s">
+    <row r="28" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B28" s="55" t="s">
         <v>323</v>
       </c>
-      <c r="C28" s="56" t="s">
-        <v>495</v>
-      </c>
-      <c r="D28" s="56" t="s">
+      <c r="C28" s="55" t="s">
+        <v>494</v>
+      </c>
+      <c r="D28" s="55" t="s">
         <v>324</v>
       </c>
-      <c r="E28" s="56" t="s">
+      <c r="E28" s="55" t="s">
         <v>46</v>
       </c>
     </row>
@@ -7650,20 +7650,20 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B30" s="56" t="s">
+    <row r="30" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B30" s="55" t="s">
         <v>325</v>
       </c>
-      <c r="C30" s="56" t="s">
-        <v>496</v>
-      </c>
-      <c r="D30" s="56" t="s">
+      <c r="C30" s="55" t="s">
+        <v>495</v>
+      </c>
+      <c r="D30" s="55" t="s">
         <v>326</v>
       </c>
-      <c r="E30" s="56" t="s">
+      <c r="E30" s="55" t="s">
         <v>46</v>
       </c>
     </row>
@@ -7708,20 +7708,20 @@
         <v>259</v>
       </c>
     </row>
-    <row r="32" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B32" s="56" t="s">
+    <row r="32" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B32" s="55" t="s">
         <v>329</v>
       </c>
-      <c r="C32" s="56" t="s">
-        <v>497</v>
-      </c>
-      <c r="D32" s="56" t="s">
+      <c r="C32" s="55" t="s">
+        <v>496</v>
+      </c>
+      <c r="D32" s="55" t="s">
         <v>330</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="55" t="s">
         <v>46</v>
       </c>
     </row>
@@ -7791,23 +7791,23 @@
       <c r="J34" s="30"/>
       <c r="R34" s="49"/>
     </row>
-    <row r="35" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B35" s="56" t="s">
+    <row r="35" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B35" s="55" t="s">
         <v>286</v>
       </c>
-      <c r="C35" s="56" t="s">
-        <v>498</v>
-      </c>
-      <c r="D35" s="56" t="s">
+      <c r="C35" s="55" t="s">
+        <v>497</v>
+      </c>
+      <c r="D35" s="55" t="s">
         <v>287</v>
       </c>
-      <c r="E35" s="56" t="s">
+      <c r="E35" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="R35" s="57"/>
+      <c r="R35" s="56"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="29"/>
@@ -8071,29 +8071,29 @@
       <c r="Q45" s="37"/>
       <c r="R45" s="2"/>
     </row>
-    <row r="46" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B46" s="56" t="s">
+    <row r="46" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B46" s="55" t="s">
         <v>335</v>
       </c>
-      <c r="C46" s="56" t="s">
-        <v>499</v>
-      </c>
-      <c r="D46" s="56" t="s">
+      <c r="C46" s="55" t="s">
+        <v>498</v>
+      </c>
+      <c r="D46" s="55" t="s">
         <v>336</v>
       </c>
-      <c r="E46" s="56" t="s">
+      <c r="E46" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="J46" s="59"/>
-      <c r="K46" s="59"/>
-      <c r="L46" s="59"/>
-      <c r="M46" s="59"/>
-      <c r="P46" s="58"/>
-      <c r="Q46" s="59"/>
-      <c r="R46" s="57"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="58"/>
+      <c r="P46" s="57"/>
+      <c r="Q46" s="58"/>
+      <c r="R46" s="56"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="29"/>
@@ -8136,23 +8136,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B48" s="56" t="s">
+    <row r="48" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B48" s="55" t="s">
         <v>339</v>
       </c>
-      <c r="C48" s="56" t="s">
-        <v>500</v>
-      </c>
-      <c r="D48" s="56" t="s">
+      <c r="C48" s="55" t="s">
+        <v>499</v>
+      </c>
+      <c r="D48" s="55" t="s">
         <v>340</v>
       </c>
-      <c r="E48" s="56" t="s">
+      <c r="E48" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="R48" s="57"/>
+      <c r="R48" s="56"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="29"/>
@@ -8195,29 +8195,29 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B50" s="56" t="s">
+    <row r="50" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B50" s="55" t="s">
         <v>341</v>
       </c>
-      <c r="C50" s="56" t="s">
-        <v>501</v>
-      </c>
-      <c r="D50" s="56" t="s">
+      <c r="C50" s="55" t="s">
+        <v>500</v>
+      </c>
+      <c r="D50" s="55" t="s">
         <v>342</v>
       </c>
-      <c r="E50" s="56" t="s">
+      <c r="E50" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="J50" s="59"/>
-      <c r="K50" s="59"/>
-      <c r="L50" s="59"/>
-      <c r="M50" s="59"/>
-      <c r="P50" s="58"/>
-      <c r="Q50" s="59"/>
-      <c r="R50" s="57"/>
+      <c r="J50" s="58"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="58"/>
+      <c r="P50" s="57"/>
+      <c r="Q50" s="58"/>
+      <c r="R50" s="56"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="29"/>
@@ -8501,23 +8501,23 @@
       </c>
       <c r="J61" s="30"/>
     </row>
-    <row r="62" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B62" s="56" t="s">
+    <row r="62" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B62" s="55" t="s">
         <v>345</v>
       </c>
-      <c r="C62" s="56" t="s">
-        <v>502</v>
-      </c>
-      <c r="D62" s="56" t="s">
+      <c r="C62" s="55" t="s">
+        <v>501</v>
+      </c>
+      <c r="D62" s="55" t="s">
         <v>346</v>
       </c>
-      <c r="E62" s="56" t="s">
+      <c r="E62" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="R62" s="57"/>
+      <c r="R62" s="56"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="29"/>
@@ -8592,7 +8592,7 @@
         <v>349</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>350</v>
@@ -8608,7 +8608,7 @@
       </c>
       <c r="C66" s="29"/>
       <c r="D66" s="29" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E66" s="29" t="s">
         <v>262</v>
@@ -8674,7 +8674,7 @@
         <v>354</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>355</v>
@@ -8690,7 +8690,7 @@
       </c>
       <c r="C69" s="29"/>
       <c r="D69" s="29" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E69" s="29" t="s">
         <v>262</v>
@@ -8732,7 +8732,7 @@
         <v>356</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>357</v>
@@ -8748,7 +8748,7 @@
       </c>
       <c r="C71" s="29"/>
       <c r="D71" s="29" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E71" s="29" t="s">
         <v>262</v>
@@ -8790,7 +8790,7 @@
         <v>358</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>359</v>
@@ -8806,7 +8806,7 @@
       </c>
       <c r="C73" s="29"/>
       <c r="D73" s="29" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E73" s="29" t="s">
         <v>262</v>
@@ -8845,10 +8845,10 @@
         <v>1</v>
       </c>
       <c r="B74" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>533</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>534</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>283</v>
@@ -8864,7 +8864,7 @@
       </c>
       <c r="C75" s="29"/>
       <c r="D75" s="29" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E75" s="29" t="s">
         <v>262</v>
@@ -8903,10 +8903,10 @@
         <v>1</v>
       </c>
       <c r="B76" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>536</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>537</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>362</v>
@@ -8922,7 +8922,7 @@
       </c>
       <c r="C77" s="29"/>
       <c r="D77" s="29" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E77" s="29" t="s">
         <v>262</v>
@@ -8964,7 +8964,7 @@
         <v>365</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>366</v>
@@ -8980,7 +8980,7 @@
       </c>
       <c r="C79" s="29"/>
       <c r="D79" s="29" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E79" s="29" t="s">
         <v>262</v>
@@ -9073,7 +9073,7 @@
         <v>44</v>
       </c>
       <c r="H82" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I82" s="29">
         <v>18</v>
@@ -9096,7 +9096,7 @@
         <v>44</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I83" s="29">
         <v>9</v>
@@ -9140,7 +9140,7 @@
         <v>44</v>
       </c>
       <c r="H85" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I85" s="29">
         <v>18</v>
@@ -9163,7 +9163,7 @@
         <v>44</v>
       </c>
       <c r="H86" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I86" s="29">
         <v>9</v>
@@ -9207,7 +9207,7 @@
         <v>44</v>
       </c>
       <c r="H88" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I88" s="29">
         <v>18</v>
@@ -9230,7 +9230,7 @@
         <v>44</v>
       </c>
       <c r="H89" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I89" s="29">
         <v>9</v>
@@ -9244,7 +9244,7 @@
         <v>367</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>368</v>
@@ -9261,7 +9261,7 @@
       </c>
       <c r="C91" s="29"/>
       <c r="D91" s="29" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E91" s="29" t="s">
         <v>262</v>
@@ -9302,7 +9302,7 @@
         <v>369</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>370</v>
@@ -9319,7 +9319,7 @@
       </c>
       <c r="C93" s="29"/>
       <c r="D93" s="29" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E93" s="29" t="s">
         <v>262</v>
@@ -9411,7 +9411,7 @@
         <v>44</v>
       </c>
       <c r="H96" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I96" s="29">
         <v>18</v>
@@ -9434,7 +9434,7 @@
         <v>44</v>
       </c>
       <c r="H97" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I97" s="29">
         <v>9</v>
@@ -9478,7 +9478,7 @@
         <v>44</v>
       </c>
       <c r="H99" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I99" s="29">
         <v>18</v>
@@ -9501,7 +9501,7 @@
         <v>44</v>
       </c>
       <c r="H100" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I100" s="29">
         <v>9</v>
@@ -9545,7 +9545,7 @@
         <v>44</v>
       </c>
       <c r="H102" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I102" s="29">
         <v>18</v>
@@ -9568,7 +9568,7 @@
         <v>44</v>
       </c>
       <c r="H103" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I103" s="29">
         <v>9</v>
@@ -9582,7 +9582,7 @@
         <v>371</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>372</v>
@@ -9599,7 +9599,7 @@
       </c>
       <c r="C105" s="29"/>
       <c r="D105" s="29" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E105" s="29" t="s">
         <v>262</v>
@@ -9691,7 +9691,7 @@
         <v>44</v>
       </c>
       <c r="H108" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I108" s="29">
         <v>18</v>
@@ -9714,7 +9714,7 @@
         <v>44</v>
       </c>
       <c r="H109" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I109" s="29">
         <v>9</v>
@@ -9758,7 +9758,7 @@
         <v>44</v>
       </c>
       <c r="H111" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I111" s="29">
         <v>18</v>
@@ -9781,7 +9781,7 @@
         <v>44</v>
       </c>
       <c r="H112" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I112" s="29">
         <v>9</v>
@@ -9825,7 +9825,7 @@
         <v>44</v>
       </c>
       <c r="H114" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I114" s="29">
         <v>18</v>
@@ -9848,7 +9848,7 @@
         <v>44</v>
       </c>
       <c r="H115" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I115" s="29">
         <v>9</v>
@@ -9862,7 +9862,7 @@
         <v>373</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>374</v>
@@ -9879,7 +9879,7 @@
       </c>
       <c r="C117" s="29"/>
       <c r="D117" s="29" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E117" s="29" t="s">
         <v>262</v>
@@ -9920,7 +9920,7 @@
         <v>375</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>376</v>
@@ -9937,7 +9937,7 @@
       </c>
       <c r="C119" s="29"/>
       <c r="D119" s="29" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E119" s="29" t="s">
         <v>262</v>
@@ -9978,7 +9978,7 @@
         <v>377</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>378</v>
@@ -9995,7 +9995,7 @@
       </c>
       <c r="C121" s="29"/>
       <c r="D121" s="29" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E121" s="29" t="s">
         <v>262</v>
@@ -10028,23 +10028,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="122" spans="1:18" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="B122" s="63" t="s">
+    <row r="122" spans="1:18" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="B122" s="62" t="s">
         <v>383</v>
       </c>
-      <c r="C122" s="63" t="s">
-        <v>580</v>
-      </c>
-      <c r="D122" s="63" t="s">
+      <c r="C122" s="62" t="s">
+        <v>579</v>
+      </c>
+      <c r="D122" s="62" t="s">
         <v>384</v>
       </c>
-      <c r="E122" s="63" t="s">
+      <c r="E122" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="J122" s="64"/>
+      <c r="J122" s="63"/>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" s="29"/>
@@ -10053,7 +10053,7 @@
       </c>
       <c r="C123" s="29"/>
       <c r="D123" s="29" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E123" s="29" t="s">
         <v>262</v>
@@ -10087,23 +10087,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="124" spans="1:18" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="B124" s="63" t="s">
+    <row r="124" spans="1:18" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="B124" s="62" t="s">
         <v>385</v>
       </c>
-      <c r="C124" s="63" t="s">
-        <v>582</v>
-      </c>
-      <c r="D124" s="63" t="s">
+      <c r="C124" s="62" t="s">
+        <v>581</v>
+      </c>
+      <c r="D124" s="62" t="s">
         <v>386</v>
       </c>
-      <c r="E124" s="63" t="s">
+      <c r="E124" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="J124" s="64"/>
+      <c r="J124" s="63"/>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125" s="29"/>
@@ -10112,7 +10112,7 @@
       </c>
       <c r="C125" s="29"/>
       <c r="D125" s="29" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E125" s="29" t="s">
         <v>262</v>
@@ -10169,23 +10169,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:18" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="B127" s="63" t="s">
+    <row r="127" spans="1:18" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="B127" s="62" t="s">
         <v>393</v>
       </c>
-      <c r="C127" s="63" t="s">
-        <v>584</v>
-      </c>
-      <c r="D127" s="63" t="s">
+      <c r="C127" s="62" t="s">
+        <v>583</v>
+      </c>
+      <c r="D127" s="62" t="s">
         <v>394</v>
       </c>
-      <c r="E127" s="63" t="s">
+      <c r="E127" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="J127" s="64"/>
+      <c r="J127" s="63"/>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A128" s="29"/>
@@ -10194,7 +10194,7 @@
       </c>
       <c r="C128" s="29"/>
       <c r="D128" s="29" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E128" s="29" t="s">
         <v>262</v>
@@ -10228,23 +10228,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="129" spans="1:18" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="B129" s="63" t="s">
+    <row r="129" spans="1:18" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="B129" s="62" t="s">
         <v>395</v>
       </c>
-      <c r="C129" s="63" t="s">
-        <v>586</v>
-      </c>
-      <c r="D129" s="63" t="s">
+      <c r="C129" s="62" t="s">
+        <v>585</v>
+      </c>
+      <c r="D129" s="62" t="s">
         <v>396</v>
       </c>
-      <c r="E129" s="63" t="s">
+      <c r="E129" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="J129" s="64"/>
+      <c r="J129" s="63"/>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130" s="29"/>
@@ -10253,7 +10253,7 @@
       </c>
       <c r="C130" s="29"/>
       <c r="D130" s="29" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E130" s="29" t="s">
         <v>262</v>
@@ -10310,23 +10310,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:18" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="B132" s="63" t="s">
+    <row r="132" spans="1:18" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="B132" s="62" t="s">
         <v>402</v>
       </c>
-      <c r="C132" s="63" t="s">
-        <v>588</v>
-      </c>
-      <c r="D132" s="63" t="s">
+      <c r="C132" s="62" t="s">
+        <v>587</v>
+      </c>
+      <c r="D132" s="62" t="s">
         <v>403</v>
       </c>
-      <c r="E132" s="63" t="s">
+      <c r="E132" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="J132" s="64"/>
+      <c r="J132" s="63"/>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133" s="29"/>
@@ -10335,7 +10335,7 @@
       </c>
       <c r="C133" s="29"/>
       <c r="D133" s="29" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E133" s="29" t="s">
         <v>262</v>
@@ -10369,23 +10369,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="134" spans="1:18" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="B134" s="63" t="s">
+    <row r="134" spans="1:18" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="B134" s="62" t="s">
         <v>404</v>
       </c>
-      <c r="C134" s="63" t="s">
-        <v>590</v>
-      </c>
-      <c r="D134" s="63" t="s">
+      <c r="C134" s="62" t="s">
+        <v>589</v>
+      </c>
+      <c r="D134" s="62" t="s">
         <v>405</v>
       </c>
-      <c r="E134" s="63" t="s">
+      <c r="E134" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="J134" s="64"/>
+      <c r="J134" s="63"/>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135" s="29"/>
@@ -10394,7 +10394,7 @@
       </c>
       <c r="C135" s="29"/>
       <c r="D135" s="29" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E135" s="29" t="s">
         <v>262</v>
@@ -10650,23 +10650,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:18" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="B146" s="63" t="s">
+    <row r="146" spans="1:18" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="B146" s="62" t="s">
         <v>408</v>
       </c>
-      <c r="C146" s="63" t="s">
-        <v>592</v>
-      </c>
-      <c r="D146" s="63" t="s">
+      <c r="C146" s="62" t="s">
+        <v>591</v>
+      </c>
+      <c r="D146" s="62" t="s">
         <v>409</v>
       </c>
-      <c r="E146" s="63" t="s">
+      <c r="E146" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="J146" s="64"/>
+      <c r="J146" s="63"/>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147" s="29"/>
@@ -10675,7 +10675,7 @@
       </c>
       <c r="C147" s="29"/>
       <c r="D147" s="29" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E147" s="29" t="s">
         <v>262</v>
@@ -10931,23 +10931,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:18" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="B158" s="63" t="s">
+    <row r="158" spans="1:18" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="B158" s="62" t="s">
         <v>410</v>
       </c>
-      <c r="C158" s="63" t="s">
-        <v>594</v>
-      </c>
-      <c r="D158" s="63" t="s">
+      <c r="C158" s="62" t="s">
+        <v>593</v>
+      </c>
+      <c r="D158" s="62" t="s">
         <v>411</v>
       </c>
-      <c r="E158" s="63" t="s">
+      <c r="E158" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="J158" s="64"/>
+      <c r="J158" s="63"/>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A159" s="29"/>
@@ -10956,7 +10956,7 @@
       </c>
       <c r="C159" s="29"/>
       <c r="D159" s="29" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E159" s="29" t="s">
         <v>262</v>
@@ -10990,23 +10990,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="160" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B160" s="54" t="s">
+    <row r="160" spans="1:18" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="B160" s="53" t="s">
         <v>412</v>
       </c>
-      <c r="C160" s="54" t="s">
-        <v>612</v>
-      </c>
-      <c r="D160" s="54" t="s">
+      <c r="C160" s="53" t="s">
+        <v>611</v>
+      </c>
+      <c r="D160" s="53" t="s">
         <v>413</v>
       </c>
-      <c r="E160" s="54" t="s">
+      <c r="E160" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J160" s="66"/>
+      <c r="J160" s="65"/>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A161" s="29"/>
@@ -11015,14 +11015,12 @@
       </c>
       <c r="C161" s="29"/>
       <c r="D161" s="29" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E161" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="F161" s="29" t="s">
-        <v>320</v>
-      </c>
+      <c r="F161" s="29"/>
       <c r="G161" s="29" t="s">
         <v>45</v>
       </c>
@@ -11063,9 +11061,7 @@
       <c r="E162" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="F162" s="29" t="s">
-        <v>414</v>
-      </c>
+      <c r="F162" s="29"/>
       <c r="G162" s="29" t="s">
         <v>44</v>
       </c>
@@ -11076,23 +11072,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B163" s="54" t="s">
+    <row r="163" spans="1:18" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="B163" s="53" t="s">
         <v>416</v>
       </c>
-      <c r="C163" s="54" t="s">
-        <v>614</v>
-      </c>
-      <c r="D163" s="54" t="s">
+      <c r="C163" s="53" t="s">
+        <v>613</v>
+      </c>
+      <c r="D163" s="53" t="s">
         <v>417</v>
       </c>
-      <c r="E163" s="54" t="s">
+      <c r="E163" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J163" s="66"/>
+      <c r="J163" s="65"/>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A164" s="29"/>
@@ -11101,14 +11097,12 @@
       </c>
       <c r="C164" s="29"/>
       <c r="D164" s="29" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E164" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="F164" s="29" t="s">
-        <v>320</v>
-      </c>
+      <c r="F164" s="29"/>
       <c r="G164" s="29" t="s">
         <v>45</v>
       </c>
@@ -11137,23 +11131,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="165" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B165" s="54" t="s">
+    <row r="165" spans="1:18" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="B165" s="53" t="s">
         <v>418</v>
       </c>
-      <c r="C165" s="54" t="s">
-        <v>616</v>
-      </c>
-      <c r="D165" s="54" t="s">
+      <c r="C165" s="53" t="s">
+        <v>615</v>
+      </c>
+      <c r="D165" s="53" t="s">
         <v>419</v>
       </c>
-      <c r="E165" s="54" t="s">
+      <c r="E165" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J165" s="66"/>
+      <c r="J165" s="65"/>
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A166" s="29"/>
@@ -11162,14 +11156,12 @@
       </c>
       <c r="C166" s="29"/>
       <c r="D166" s="29" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E166" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="F166" s="29" t="s">
-        <v>320</v>
-      </c>
+      <c r="F166" s="29"/>
       <c r="G166" s="29" t="s">
         <v>45</v>
       </c>
@@ -11198,23 +11190,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="167" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B167" s="54" t="s">
+    <row r="167" spans="1:18" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="B167" s="53" t="s">
         <v>420</v>
       </c>
-      <c r="C167" s="54" t="s">
-        <v>618</v>
-      </c>
-      <c r="D167" s="54" t="s">
+      <c r="C167" s="53" t="s">
+        <v>617</v>
+      </c>
+      <c r="D167" s="53" t="s">
         <v>421</v>
       </c>
-      <c r="E167" s="54" t="s">
+      <c r="E167" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J167" s="66"/>
+      <c r="J167" s="65"/>
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A168" s="29"/>
@@ -11223,14 +11215,12 @@
       </c>
       <c r="C168" s="29"/>
       <c r="D168" s="29" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E168" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="F168" s="29" t="s">
-        <v>320</v>
-      </c>
+      <c r="F168" s="29"/>
       <c r="G168" s="29" t="s">
         <v>45</v>
       </c>
@@ -11259,23 +11249,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="169" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B169" s="54" t="s">
+    <row r="169" spans="1:18" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="B169" s="53" t="s">
         <v>422</v>
       </c>
-      <c r="C169" s="54" t="s">
-        <v>620</v>
-      </c>
-      <c r="D169" s="54" t="s">
+      <c r="C169" s="53" t="s">
+        <v>619</v>
+      </c>
+      <c r="D169" s="53" t="s">
         <v>423</v>
       </c>
-      <c r="E169" s="54" t="s">
+      <c r="E169" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J169" s="66"/>
+      <c r="J169" s="65"/>
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A170" s="29"/>
@@ -11284,14 +11274,12 @@
       </c>
       <c r="C170" s="29"/>
       <c r="D170" s="29" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E170" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="F170" s="29" t="s">
-        <v>320</v>
-      </c>
+      <c r="F170" s="29"/>
       <c r="G170" s="29" t="s">
         <v>45</v>
       </c>
@@ -11332,9 +11320,7 @@
       <c r="E171" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="F171" s="29" t="s">
-        <v>424</v>
-      </c>
+      <c r="F171" s="29"/>
       <c r="G171" s="29" t="s">
         <v>44</v>
       </c>
@@ -11355,9 +11341,7 @@
       <c r="E172" s="29" t="s">
         <v>427</v>
       </c>
-      <c r="F172" s="29" t="s">
-        <v>426</v>
-      </c>
+      <c r="F172" s="29"/>
       <c r="G172" s="29" t="s">
         <v>44</v>
       </c>
@@ -11380,9 +11364,7 @@
       <c r="E173" s="29" t="s">
         <v>429</v>
       </c>
-      <c r="F173" s="29" t="s">
-        <v>428</v>
-      </c>
+      <c r="F173" s="29"/>
       <c r="G173" s="29" t="s">
         <v>44</v>
       </c>
@@ -11393,23 +11375,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="174" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B174" s="54" t="s">
+    <row r="174" spans="1:18" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="B174" s="53" t="s">
         <v>430</v>
       </c>
-      <c r="C174" s="54" t="s">
-        <v>622</v>
-      </c>
-      <c r="D174" s="54" t="s">
+      <c r="C174" s="53" t="s">
+        <v>621</v>
+      </c>
+      <c r="D174" s="53" t="s">
         <v>431</v>
       </c>
-      <c r="E174" s="54" t="s">
+      <c r="E174" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J174" s="66"/>
+      <c r="J174" s="65"/>
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A175" s="29"/>
@@ -11418,14 +11400,12 @@
       </c>
       <c r="C175" s="29"/>
       <c r="D175" s="29" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E175" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="F175" s="29" t="s">
-        <v>320</v>
-      </c>
+      <c r="F175" s="29"/>
       <c r="G175" s="29" t="s">
         <v>45</v>
       </c>
@@ -11466,9 +11446,7 @@
       <c r="E176" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F176" s="29" t="s">
-        <v>432</v>
-      </c>
+      <c r="F176" s="29"/>
       <c r="G176" s="29" t="s">
         <v>44</v>
       </c>
@@ -11479,23 +11457,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="177" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B177" s="54" t="s">
+    <row r="177" spans="1:18" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="B177" s="53" t="s">
         <v>433</v>
       </c>
-      <c r="C177" s="54" t="s">
-        <v>624</v>
-      </c>
-      <c r="D177" s="54" t="s">
+      <c r="C177" s="53" t="s">
+        <v>623</v>
+      </c>
+      <c r="D177" s="53" t="s">
         <v>434</v>
       </c>
-      <c r="E177" s="54" t="s">
+      <c r="E177" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J177" s="66"/>
+      <c r="J177" s="65"/>
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A178" s="29"/>
@@ -11504,14 +11482,12 @@
       </c>
       <c r="C178" s="29"/>
       <c r="D178" s="29" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E178" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="F178" s="29" t="s">
-        <v>320</v>
-      </c>
+      <c r="F178" s="29"/>
       <c r="G178" s="29" t="s">
         <v>45</v>
       </c>
@@ -11540,23 +11516,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="179" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B179" s="54" t="s">
+    <row r="179" spans="1:18" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="B179" s="53" t="s">
         <v>435</v>
       </c>
-      <c r="C179" s="54" t="s">
-        <v>626</v>
-      </c>
-      <c r="D179" s="54" t="s">
+      <c r="C179" s="53" t="s">
+        <v>625</v>
+      </c>
+      <c r="D179" s="53" t="s">
         <v>436</v>
       </c>
-      <c r="E179" s="54" t="s">
+      <c r="E179" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J179" s="66"/>
+      <c r="J179" s="65"/>
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A180" s="29"/>
@@ -11565,14 +11541,12 @@
       </c>
       <c r="C180" s="29"/>
       <c r="D180" s="29" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E180" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="F180" s="29" t="s">
-        <v>320</v>
-      </c>
+      <c r="F180" s="29"/>
       <c r="G180" s="29" t="s">
         <v>45</v>
       </c>
@@ -11601,23 +11575,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="181" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B181" s="54" t="s">
+    <row r="181" spans="1:18" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="B181" s="53" t="s">
         <v>465</v>
       </c>
-      <c r="C181" s="54" t="s">
-        <v>628</v>
-      </c>
-      <c r="D181" s="54" t="s">
+      <c r="C181" s="53" t="s">
+        <v>627</v>
+      </c>
+      <c r="D181" s="53" t="s">
         <v>466</v>
       </c>
-      <c r="E181" s="54" t="s">
+      <c r="E181" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J181" s="66"/>
+      <c r="J181" s="65"/>
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A182" s="29"/>
@@ -11626,14 +11600,12 @@
       </c>
       <c r="C182" s="29"/>
       <c r="D182" s="29" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E182" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="F182" s="29" t="s">
-        <v>320</v>
-      </c>
+      <c r="F182" s="29"/>
       <c r="G182" s="29" t="s">
         <v>45</v>
       </c>
@@ -11662,23 +11634,23 @@
         <v>259</v>
       </c>
     </row>
-    <row r="183" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B183" s="54" t="s">
+    <row r="183" spans="1:18" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="B183" s="53" t="s">
         <v>467</v>
       </c>
-      <c r="C183" s="54" t="s">
-        <v>630</v>
-      </c>
-      <c r="D183" s="54" t="s">
+      <c r="C183" s="53" t="s">
+        <v>629</v>
+      </c>
+      <c r="D183" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E183" s="54" t="s">
+      <c r="E183" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J183" s="66"/>
+      <c r="J183" s="65"/>
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A184" s="29"/>
@@ -11687,14 +11659,12 @@
       </c>
       <c r="C184" s="29"/>
       <c r="D184" s="29" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E184" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="F184" s="29" t="s">
-        <v>320</v>
-      </c>
+      <c r="F184" s="29"/>
       <c r="G184" s="29" t="s">
         <v>45</v>
       </c>
@@ -11735,9 +11705,7 @@
       <c r="E185" s="29" t="s">
         <v>470</v>
       </c>
-      <c r="F185" s="29" t="s">
-        <v>469</v>
-      </c>
+      <c r="F185" s="29"/>
       <c r="G185" s="29" t="s">
         <v>44</v>
       </c>
@@ -11768,8 +11736,8 @@
   <dimension ref="A1:M89"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12379,34 +12347,34 @@
       <c r="L20" s="38"/>
       <c r="M20" s="38"/>
     </row>
-    <row r="21" spans="1:13" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="61" t="s">
+    <row r="21" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="60" t="s">
         <v>282</v>
       </c>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="60" t="s">
         <v>282</v>
       </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61" t="s">
+      <c r="C21" s="60"/>
+      <c r="D21" s="60" t="s">
         <v>280</v>
       </c>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61" t="s">
+      <c r="E21" s="60"/>
+      <c r="F21" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="61" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" s="61" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="61" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
+      <c r="G21" s="60" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="60" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="60" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
     </row>
     <row r="22" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35" t="s">
@@ -12415,26 +12383,26 @@
       <c r="B22" s="35" t="s">
         <v>483</v>
       </c>
-      <c r="D22" s="53" t="s">
+      <c r="D22" s="52" t="s">
         <v>477</v>
       </c>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53" t="s">
+      <c r="E22" s="52"/>
+      <c r="F22" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
+      <c r="G22" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
     </row>
     <row r="23" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35" t="s">
@@ -12443,26 +12411,26 @@
       <c r="B23" s="35" t="s">
         <v>484</v>
       </c>
-      <c r="D23" s="53" t="s">
+      <c r="D23" s="52" t="s">
         <v>478</v>
       </c>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53" t="s">
+      <c r="E23" s="52"/>
+      <c r="F23" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
+      <c r="G23" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
     </row>
     <row r="24" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35" t="s">
@@ -12471,26 +12439,26 @@
       <c r="B24" s="35" t="s">
         <v>485</v>
       </c>
-      <c r="D24" s="53" t="s">
+      <c r="D24" s="52" t="s">
         <v>479</v>
       </c>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53" t="s">
+      <c r="E24" s="52"/>
+      <c r="F24" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
+      <c r="G24" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
     </row>
     <row r="25" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="s">
@@ -12499,26 +12467,26 @@
       <c r="B25" s="35" t="s">
         <v>486</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D25" s="52" t="s">
         <v>480</v>
       </c>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53" t="s">
+      <c r="E25" s="52"/>
+      <c r="F25" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="53"/>
+      <c r="G25" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
     </row>
     <row r="26" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="35" t="s">
@@ -12527,26 +12495,26 @@
       <c r="B26" s="35" t="s">
         <v>487</v>
       </c>
-      <c r="D26" s="53" t="s">
+      <c r="D26" s="52" t="s">
         <v>481</v>
       </c>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53" t="s">
+      <c r="E26" s="52"/>
+      <c r="F26" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
+      <c r="G26" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="52"/>
     </row>
     <row r="27" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="35" t="s">
@@ -12555,26 +12523,26 @@
       <c r="B27" s="35" t="s">
         <v>488</v>
       </c>
-      <c r="D27" s="53" t="s">
+      <c r="D27" s="52" t="s">
         <v>482</v>
       </c>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53" t="s">
+      <c r="E27" s="52"/>
+      <c r="F27" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="G27" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="H27" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
+      <c r="G27" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
     </row>
     <row r="28" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
@@ -12586,1010 +12554,1010 @@
       <c r="D28" s="35" t="s">
         <v>279</v>
       </c>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53" t="s">
+      <c r="E28" s="52"/>
+      <c r="F28" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="G28" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53"/>
-    </row>
-    <row r="29" spans="1:13" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="56" t="s">
+      <c r="G28" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+    </row>
+    <row r="29" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="55" t="s">
+        <v>502</v>
+      </c>
+      <c r="B29" s="55" t="s">
+        <v>502</v>
+      </c>
+      <c r="D29" s="55" t="s">
         <v>503</v>
       </c>
-      <c r="B29" s="56" t="s">
-        <v>503</v>
-      </c>
-      <c r="D29" s="56" t="s">
+      <c r="E29" s="56"/>
+      <c r="F29" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+    </row>
+    <row r="30" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="55" t="s">
         <v>504</v>
       </c>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57" t="s">
+      <c r="B30" s="55" t="s">
+        <v>504</v>
+      </c>
+      <c r="D30" s="55" t="s">
+        <v>505</v>
+      </c>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G29" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="57"/>
-    </row>
-    <row r="30" spans="1:13" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="56" t="s">
-        <v>505</v>
-      </c>
-      <c r="B30" s="56" t="s">
-        <v>505</v>
-      </c>
-      <c r="D30" s="56" t="s">
+      <c r="G30" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+    </row>
+    <row r="31" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="55" t="s">
         <v>506</v>
       </c>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57" t="s">
+      <c r="B31" s="55" t="s">
+        <v>506</v>
+      </c>
+      <c r="D31" s="55" t="s">
+        <v>507</v>
+      </c>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G30" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I30" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-    </row>
-    <row r="31" spans="1:13" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="56" t="s">
-        <v>507</v>
-      </c>
-      <c r="B31" s="56" t="s">
-        <v>507</v>
-      </c>
-      <c r="D31" s="56" t="s">
+      <c r="G31" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+    </row>
+    <row r="32" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="55" t="s">
         <v>508</v>
       </c>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57" t="s">
+      <c r="B32" s="55" t="s">
+        <v>508</v>
+      </c>
+      <c r="D32" s="55" t="s">
+        <v>509</v>
+      </c>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G31" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H31" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I31" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="57"/>
-    </row>
-    <row r="32" spans="1:13" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="56" t="s">
-        <v>509</v>
-      </c>
-      <c r="B32" s="56" t="s">
-        <v>509</v>
-      </c>
-      <c r="D32" s="56" t="s">
+      <c r="G32" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="55" t="s">
         <v>510</v>
       </c>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57" t="s">
+      <c r="B33" s="55" t="s">
+        <v>510</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>511</v>
+      </c>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" s="57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="56" t="s">
-        <v>511</v>
-      </c>
-      <c r="B33" s="56" t="s">
-        <v>511</v>
-      </c>
-      <c r="D33" s="56" t="s">
+      <c r="G33" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="55" t="s">
         <v>512</v>
       </c>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57" t="s">
+      <c r="B34" s="55" t="s">
+        <v>512</v>
+      </c>
+      <c r="D34" s="55" t="s">
+        <v>513</v>
+      </c>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G33" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" s="57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="56" t="s">
-        <v>513</v>
-      </c>
-      <c r="B34" s="56" t="s">
-        <v>513</v>
-      </c>
-      <c r="D34" s="56" t="s">
+      <c r="G34" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="55" t="s">
         <v>514</v>
       </c>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57" t="s">
+      <c r="B35" s="55" t="s">
+        <v>514</v>
+      </c>
+      <c r="D35" s="55" t="s">
+        <v>515</v>
+      </c>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G34" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" s="57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="56" t="s">
-        <v>515</v>
-      </c>
-      <c r="B35" s="56" t="s">
-        <v>515</v>
-      </c>
-      <c r="D35" s="56" t="s">
+      <c r="G35" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="55" t="s">
         <v>516</v>
       </c>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57" t="s">
+      <c r="B36" s="55" t="s">
+        <v>516</v>
+      </c>
+      <c r="D36" s="55" t="s">
+        <v>517</v>
+      </c>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" s="57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="56" t="s">
-        <v>517</v>
-      </c>
-      <c r="B36" s="56" t="s">
-        <v>517</v>
-      </c>
-      <c r="D36" s="56" t="s">
+      <c r="G36" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="55" t="s">
         <v>518</v>
       </c>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57" t="s">
+      <c r="B37" s="55" t="s">
+        <v>518</v>
+      </c>
+      <c r="D37" s="55" t="s">
+        <v>519</v>
+      </c>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G36" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" s="57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="56" t="s">
-        <v>519</v>
-      </c>
-      <c r="B37" s="56" t="s">
-        <v>519</v>
-      </c>
-      <c r="D37" s="56" t="s">
+      <c r="G37" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="55" t="s">
         <v>520</v>
       </c>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57" t="s">
+      <c r="B38" s="55" t="s">
+        <v>520</v>
+      </c>
+      <c r="D38" s="55" t="s">
+        <v>521</v>
+      </c>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I37" s="57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="56" t="s">
-        <v>521</v>
-      </c>
-      <c r="B38" s="56" t="s">
-        <v>521</v>
-      </c>
-      <c r="D38" s="56" t="s">
+      <c r="G38" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="55" t="s">
         <v>522</v>
       </c>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57" t="s">
+      <c r="B39" s="55" t="s">
+        <v>522</v>
+      </c>
+      <c r="D39" s="55" t="s">
+        <v>523</v>
+      </c>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G38" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" s="57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="56" t="s">
-        <v>523</v>
-      </c>
-      <c r="B39" s="56" t="s">
-        <v>523</v>
-      </c>
-      <c r="D39" s="56" t="s">
-        <v>524</v>
-      </c>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="G39" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" s="57" t="b">
+      <c r="G39" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="56" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
+        <v>553</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>553</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>554</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="F40" s="62" t="s">
+      <c r="F40" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G40" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" s="62" t="b">
+      <c r="G40" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>556</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>556</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>557</v>
-      </c>
-      <c r="F41" s="62" t="s">
+      <c r="F41" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G41" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I41" s="62" t="b">
+      <c r="G41" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>558</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>559</v>
-      </c>
-      <c r="F42" s="62" t="s">
+      <c r="F42" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G42" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" s="62" t="b">
+      <c r="G42" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>560</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>560</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>561</v>
-      </c>
-      <c r="F43" s="62" t="s">
+      <c r="F43" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G43" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43" s="62" t="b">
+      <c r="G43" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>562</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="F44" s="62" t="s">
+      <c r="F44" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H44" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I44" s="62" t="b">
+      <c r="G44" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>564</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>564</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>565</v>
-      </c>
-      <c r="F45" s="62" t="s">
+      <c r="F45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G45" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I45" s="62" t="b">
+      <c r="G45" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>566</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>567</v>
-      </c>
-      <c r="F46" s="62" t="s">
+      <c r="F46" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G46" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H46" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I46" s="62" t="b">
+      <c r="G46" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>568</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>569</v>
-      </c>
-      <c r="F47" s="62" t="s">
+      <c r="F47" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G47" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H47" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I47" s="62" t="b">
+      <c r="G47" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>570</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>571</v>
-      </c>
-      <c r="F48" s="62" t="s">
+      <c r="F48" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G48" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H48" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I48" s="62" t="b">
+      <c r="G48" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>573</v>
-      </c>
-      <c r="F49" s="62" t="s">
+      <c r="F49" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G49" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H49" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49" s="62" t="b">
+      <c r="G49" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>574</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>574</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>575</v>
-      </c>
-      <c r="F50" s="62" t="s">
+      <c r="F50" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G50" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H50" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I50" s="62" t="b">
+      <c r="G50" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>576</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="F51" s="62" t="s">
+      <c r="F51" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G51" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H51" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I51" s="62" t="b">
+      <c r="G51" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" s="61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>579</v>
-      </c>
-      <c r="F52" s="62" t="s">
+      <c r="F52" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G52" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H52" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I52" s="62" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="63" t="s">
+      <c r="G52" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" s="61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="62" t="s">
+        <v>595</v>
+      </c>
+      <c r="B53" s="62" t="s">
+        <v>595</v>
+      </c>
+      <c r="D53" s="62" t="s">
         <v>596</v>
       </c>
-      <c r="B53" s="63" t="s">
-        <v>596</v>
-      </c>
-      <c r="D53" s="63" t="s">
+      <c r="F53" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="G53" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" s="64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="62" t="s">
         <v>597</v>
       </c>
-      <c r="F53" s="65" t="s">
+      <c r="B54" s="62" t="s">
+        <v>597</v>
+      </c>
+      <c r="D54" s="62" t="s">
+        <v>598</v>
+      </c>
+      <c r="F54" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="G53" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="H53" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="I53" s="65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="63" t="s">
-        <v>598</v>
-      </c>
-      <c r="B54" s="63" t="s">
-        <v>598</v>
-      </c>
-      <c r="D54" s="63" t="s">
+      <c r="G54" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" s="64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="62" t="s">
         <v>599</v>
       </c>
-      <c r="F54" s="65" t="s">
+      <c r="B55" s="62" t="s">
+        <v>599</v>
+      </c>
+      <c r="D55" s="62" t="s">
+        <v>600</v>
+      </c>
+      <c r="F55" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="G54" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="H54" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="I54" s="65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="63" t="s">
-        <v>600</v>
-      </c>
-      <c r="B55" s="63" t="s">
-        <v>600</v>
-      </c>
-      <c r="D55" s="63" t="s">
+      <c r="G55" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" s="64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="62" t="s">
         <v>601</v>
       </c>
-      <c r="F55" s="65" t="s">
+      <c r="B56" s="62" t="s">
+        <v>601</v>
+      </c>
+      <c r="D56" s="62" t="s">
+        <v>602</v>
+      </c>
+      <c r="F56" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="G55" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="H55" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="I55" s="65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="63" t="s">
-        <v>602</v>
-      </c>
-      <c r="B56" s="63" t="s">
-        <v>602</v>
-      </c>
-      <c r="D56" s="63" t="s">
+      <c r="G56" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I56" s="64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="62" t="s">
         <v>603</v>
       </c>
-      <c r="F56" s="65" t="s">
+      <c r="B57" s="62" t="s">
+        <v>603</v>
+      </c>
+      <c r="D57" s="62" t="s">
+        <v>604</v>
+      </c>
+      <c r="F57" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="G56" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="H56" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="I56" s="65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="63" t="s">
-        <v>604</v>
-      </c>
-      <c r="B57" s="63" t="s">
-        <v>604</v>
-      </c>
-      <c r="D57" s="63" t="s">
+      <c r="G57" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" s="64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="62" t="s">
         <v>605</v>
       </c>
-      <c r="F57" s="65" t="s">
+      <c r="B58" s="62" t="s">
+        <v>605</v>
+      </c>
+      <c r="D58" s="62" t="s">
+        <v>606</v>
+      </c>
+      <c r="F58" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="G57" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="H57" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="I57" s="65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="63" t="s">
-        <v>606</v>
-      </c>
-      <c r="B58" s="63" t="s">
-        <v>606</v>
-      </c>
-      <c r="D58" s="63" t="s">
+      <c r="G58" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" s="64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="62" t="s">
         <v>607</v>
       </c>
-      <c r="F58" s="65" t="s">
+      <c r="B59" s="62" t="s">
+        <v>607</v>
+      </c>
+      <c r="D59" s="62" t="s">
+        <v>608</v>
+      </c>
+      <c r="F59" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="G58" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="H58" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="I58" s="65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="63" t="s">
-        <v>608</v>
-      </c>
-      <c r="B59" s="63" t="s">
-        <v>608</v>
-      </c>
-      <c r="D59" s="63" t="s">
+      <c r="G59" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" s="64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="62" t="s">
         <v>609</v>
       </c>
-      <c r="F59" s="65" t="s">
+      <c r="B60" s="62" t="s">
+        <v>609</v>
+      </c>
+      <c r="D60" s="62" t="s">
+        <v>610</v>
+      </c>
+      <c r="F60" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="G59" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="H59" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="I59" s="65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="63" t="s">
-        <v>610</v>
-      </c>
-      <c r="B60" s="63" t="s">
-        <v>610</v>
-      </c>
-      <c r="D60" s="63" t="s">
-        <v>611</v>
-      </c>
-      <c r="F60" s="65" t="s">
+      <c r="G60" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" s="64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="53" t="s">
+        <v>631</v>
+      </c>
+      <c r="B61" s="53" t="s">
+        <v>631</v>
+      </c>
+      <c r="D61" s="53" t="s">
+        <v>632</v>
+      </c>
+      <c r="F61" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G60" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="H60" s="65" t="b">
-        <v>1</v>
-      </c>
-      <c r="I60" s="65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="54" t="s">
-        <v>632</v>
-      </c>
-      <c r="B61" s="54" t="s">
-        <v>632</v>
-      </c>
-      <c r="D61" s="54" t="s">
+      <c r="G61" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" s="54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="53" t="s">
         <v>633</v>
       </c>
-      <c r="F61" s="55" t="s">
+      <c r="B62" s="53" t="s">
+        <v>633</v>
+      </c>
+      <c r="D62" s="53" t="s">
+        <v>634</v>
+      </c>
+      <c r="F62" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G61" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H61" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I61" s="55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="54" t="s">
-        <v>634</v>
-      </c>
-      <c r="B62" s="54" t="s">
-        <v>634</v>
-      </c>
-      <c r="D62" s="54" t="s">
+      <c r="G62" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H62" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" s="54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="53" t="s">
         <v>635</v>
       </c>
-      <c r="F62" s="55" t="s">
+      <c r="B63" s="53" t="s">
+        <v>635</v>
+      </c>
+      <c r="D63" s="53" t="s">
+        <v>636</v>
+      </c>
+      <c r="F63" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G62" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H62" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I62" s="55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="54" t="s">
-        <v>636</v>
-      </c>
-      <c r="B63" s="54" t="s">
-        <v>636</v>
-      </c>
-      <c r="D63" s="54" t="s">
+      <c r="G63" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H63" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" s="54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="53" t="s">
         <v>637</v>
       </c>
-      <c r="F63" s="55" t="s">
+      <c r="B64" s="53" t="s">
+        <v>637</v>
+      </c>
+      <c r="D64" s="53" t="s">
+        <v>638</v>
+      </c>
+      <c r="F64" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G63" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H63" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I63" s="55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="54" t="s">
-        <v>638</v>
-      </c>
-      <c r="B64" s="54" t="s">
-        <v>638</v>
-      </c>
-      <c r="D64" s="54" t="s">
+      <c r="G64" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H64" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" s="54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="53" t="s">
         <v>639</v>
       </c>
-      <c r="F64" s="55" t="s">
+      <c r="B65" s="53" t="s">
+        <v>639</v>
+      </c>
+      <c r="D65" s="53" t="s">
+        <v>640</v>
+      </c>
+      <c r="F65" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G64" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H64" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I64" s="55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="54" t="s">
-        <v>640</v>
-      </c>
-      <c r="B65" s="54" t="s">
-        <v>640</v>
-      </c>
-      <c r="D65" s="54" t="s">
+      <c r="G65" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H65" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" s="54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="53" t="s">
         <v>641</v>
       </c>
-      <c r="F65" s="55" t="s">
+      <c r="B66" s="53" t="s">
+        <v>641</v>
+      </c>
+      <c r="D66" s="53" t="s">
+        <v>642</v>
+      </c>
+      <c r="F66" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G65" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H65" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I65" s="55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="54" t="s">
-        <v>642</v>
-      </c>
-      <c r="B66" s="54" t="s">
-        <v>642</v>
-      </c>
-      <c r="D66" s="54" t="s">
+      <c r="G66" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I66" s="54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="53" t="s">
         <v>643</v>
       </c>
-      <c r="F66" s="55" t="s">
+      <c r="B67" s="53" t="s">
+        <v>643</v>
+      </c>
+      <c r="D67" s="53" t="s">
+        <v>644</v>
+      </c>
+      <c r="F67" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G66" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H66" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I66" s="55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="54" t="s">
-        <v>644</v>
-      </c>
-      <c r="B67" s="54" t="s">
-        <v>644</v>
-      </c>
-      <c r="D67" s="54" t="s">
+      <c r="G67" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H67" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" s="54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="53" t="s">
         <v>645</v>
       </c>
-      <c r="F67" s="55" t="s">
+      <c r="B68" s="53" t="s">
+        <v>645</v>
+      </c>
+      <c r="D68" s="53" t="s">
+        <v>646</v>
+      </c>
+      <c r="F68" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G67" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H67" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I67" s="55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="B68" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D68" s="54" t="s">
+      <c r="G68" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H68" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I68" s="54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="53" t="s">
         <v>647</v>
       </c>
-      <c r="F68" s="55" t="s">
+      <c r="B69" s="53" t="s">
+        <v>647</v>
+      </c>
+      <c r="D69" s="53" t="s">
+        <v>648</v>
+      </c>
+      <c r="F69" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G68" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H68" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I68" s="55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="54" t="s">
-        <v>648</v>
-      </c>
-      <c r="B69" s="54" t="s">
-        <v>648</v>
-      </c>
-      <c r="D69" s="54" t="s">
+      <c r="G69" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H69" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I69" s="54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="53" t="s">
         <v>649</v>
       </c>
-      <c r="F69" s="55" t="s">
+      <c r="B70" s="53" t="s">
+        <v>649</v>
+      </c>
+      <c r="D70" s="53" t="s">
+        <v>650</v>
+      </c>
+      <c r="F70" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G69" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H69" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I69" s="55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="54" t="s">
-        <v>650</v>
-      </c>
-      <c r="B70" s="54" t="s">
-        <v>650</v>
-      </c>
-      <c r="D70" s="54" t="s">
-        <v>651</v>
-      </c>
-      <c r="F70" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="G70" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H70" s="55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I70" s="55" t="b">
+      <c r="G70" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H70" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I70" s="54" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>